<commit_message>
*** empty log message ***
</commit_message>
<xml_diff>
--- a/Documentation/management/osu/deployed_services.xlsx
+++ b/Documentation/management/osu/deployed_services.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="480" yWindow="75" windowWidth="19995" windowHeight="14820"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="services" sheetId="1" r:id="rId1"/>
+    <sheet name="other ports" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="57">
   <si>
     <t>cagrid01.bmi.ohio-state.edu:8080</t>
   </si>
@@ -169,6 +169,24 @@
   </si>
   <si>
     <t>training.cagrid.org:7443</t>
+  </si>
+  <si>
+    <t>usage.cagrid.org:55555</t>
+  </si>
+  <si>
+    <t>introduce</t>
+  </si>
+  <si>
+    <t>Protocol</t>
+  </si>
+  <si>
+    <t>UDP</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>introduce stats collecting</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1070,7 @@
   <dimension ref="A2:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1840,12 +1858,54 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="54.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A1" s="31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="14.25" thickTop="1" thickBot="1">
+      <c r="A3" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
updated for new training deployment
</commit_message>
<xml_diff>
--- a/Documentation/management/osu/deployed_services.xlsx
+++ b/Documentation/management/osu/deployed_services.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="19995" windowHeight="14820"/>
+    <workbookView xWindow="480" yWindow="72" windowWidth="19992" windowHeight="14616"/>
   </bookViews>
   <sheets>
     <sheet name="services" sheetId="1" r:id="rId1"/>
     <sheet name="other ports" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="122">
   <si>
     <t>cagrid01.bmi.ohio-state.edu:8080</t>
   </si>
@@ -273,16 +273,138 @@
   </si>
   <si>
     <t>dorian.cagrid.org is dorian.bmi.ohio-state.edu</t>
+  </si>
+  <si>
+    <t>caGrid 1.2 Training</t>
+  </si>
+  <si>
+    <t>slavegts.training.cagrid.org:8443</t>
+  </si>
+  <si>
+    <t>training</t>
+  </si>
+  <si>
+    <t>VM</t>
+  </si>
+  <si>
+    <t>CDS</t>
+  </si>
+  <si>
+    <t>training02 has been CNAMEd to VM06</t>
+  </si>
+  <si>
+    <t>training03 has been CNAMEd to VM05</t>
+  </si>
+  <si>
+    <t>Portal</t>
+  </si>
+  <si>
+    <t>trainingvm01.bmi.ohio-state.edu</t>
+  </si>
+  <si>
+    <t>trainingvm07.bmi.ohio-state.edu</t>
+  </si>
+  <si>
+    <t>trainingvm02.bmi.ohio-state.edu</t>
+  </si>
+  <si>
+    <t>trainingvm05.bmi.ohio-state.edu</t>
+  </si>
+  <si>
+    <t>trainingvm06.bmi.ohio-state.edu</t>
+  </si>
+  <si>
+    <t>trainingvm03.bmi.ohio-state.edu</t>
+  </si>
+  <si>
+    <t>VM Server</t>
+  </si>
+  <si>
+    <t>cagrid06.bmi.ohio-state.edu</t>
+  </si>
+  <si>
+    <t>cagrid07.bmi.ohio-state.edu</t>
+  </si>
+  <si>
+    <t>cagrid08.bmi.ohio-state.edu</t>
+  </si>
+  <si>
+    <t>cagrid09.bmi.ohio-state.edu</t>
+  </si>
+  <si>
+    <t>cagrid10.bmi.ohio-state.edu</t>
+  </si>
+  <si>
+    <t>4,5</t>
+  </si>
+  <si>
+    <t>6,7</t>
+  </si>
+  <si>
+    <t>Authn</t>
+  </si>
+  <si>
+    <t>index.training.cagrid.org:8080/6080</t>
+  </si>
+  <si>
+    <t>grouper.training.cagrid.org:8443/6443</t>
+  </si>
+  <si>
+    <t>dorian.training.cagrid.org:8443/6443</t>
+  </si>
+  <si>
+    <t>mastergts.training.cagrid.org:8443/6442</t>
+  </si>
+  <si>
+    <t>cds.training.cagrid.org:8443/6442</t>
+  </si>
+  <si>
+    <t>evs.training.cagrid.org:8080/6080</t>
+  </si>
+  <si>
+    <t>workflow.training.cagrid.org:8443/6443</t>
+  </si>
+  <si>
+    <t>fqp.training.cagrid.org:8443/6443</t>
+  </si>
+  <si>
+    <t>gme.training.cagrid.org:8080/6080</t>
+  </si>
+  <si>
+    <t>cadsr.training.cagrid.org:8080/6080</t>
+  </si>
+  <si>
+    <t>portal.training.cagrid.org:443</t>
+  </si>
+  <si>
+    <t>1.5.0_14</t>
+  </si>
+  <si>
+    <t>N/A (dorian.bmi.ohio-state.edu)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -321,8 +443,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -340,8 +468,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -760,15 +900,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -783,7 +984,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -802,12 +1002,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -827,15 +1027,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -844,86 +1044,274 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="24" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -1223,88 +1611,90 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:P57"/>
+  <dimension ref="A2:S81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="54.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" customWidth="1"/>
-    <col min="8" max="8" width="7" customWidth="1"/>
-    <col min="9" max="9" width="4.85546875" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" customWidth="1"/>
-    <col min="12" max="12" width="7.42578125" customWidth="1"/>
-    <col min="13" max="13" width="5.28515625" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" customWidth="1"/>
-    <col min="16" max="16" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="54.5546875" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" customWidth="1"/>
+    <col min="6" max="6" width="29.109375" customWidth="1"/>
+    <col min="7" max="7" width="6.5546875" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" customWidth="1"/>
+    <col min="9" max="9" width="7" customWidth="1"/>
+    <col min="10" max="10" width="4.88671875" customWidth="1"/>
+    <col min="11" max="11" width="5.44140625" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" customWidth="1"/>
+    <col min="13" max="13" width="7.44140625" customWidth="1"/>
+    <col min="14" max="14" width="5.33203125" customWidth="1"/>
+    <col min="15" max="15" width="9.5546875" customWidth="1"/>
+    <col min="16" max="16" width="13.88671875" customWidth="1"/>
+    <col min="17" max="17" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="16.5" thickBot="1">
+    <row r="2" spans="1:17" ht="16.2" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:17" s="1" customFormat="1" ht="16.8" thickTop="1" thickBot="1">
+      <c r="A3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18"/>
+      <c r="G3" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="H3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="I3" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="J3" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="K3" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="L3" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="M3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="18" t="s">
+      <c r="N3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="18" t="s">
+      <c r="O3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="18" t="s">
+      <c r="P3" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="18" t="s">
+      <c r="Q3" s="17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="14.25" thickTop="1" thickBot="1">
+    <row r="4" spans="1:17" ht="14.4" thickTop="1" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1320,25 +1710,26 @@
       <c r="E4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="O4" s="37"/>
-      <c r="P4" s="38"/>
-    </row>
-    <row r="5" spans="1:16" ht="13.5" thickBot="1">
+      <c r="F4" s="153"/>
+      <c r="G4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="37"/>
+    </row>
+    <row r="5" spans="1:17" ht="13.8" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1354,23 +1745,24 @@
       <c r="E5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="O5" s="25"/>
-      <c r="P5" s="26"/>
-    </row>
-    <row r="6" spans="1:16" ht="13.5" thickBot="1">
+      <c r="F5" s="154"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="25"/>
+    </row>
+    <row r="6" spans="1:17" ht="13.8" thickBot="1">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1386,21 +1778,22 @@
       <c r="E6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="O6" s="25"/>
-      <c r="P6" s="26"/>
-    </row>
-    <row r="7" spans="1:16" ht="13.5" thickBot="1">
+      <c r="F6" s="154"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="25"/>
+    </row>
+    <row r="7" spans="1:17" ht="13.8" thickBot="1">
       <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
@@ -1416,21 +1809,22 @@
       <c r="E7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="O7" s="25"/>
-      <c r="P7" s="26"/>
-    </row>
-    <row r="8" spans="1:16" ht="13.5" thickBot="1">
+      <c r="F7" s="154"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="25"/>
+    </row>
+    <row r="8" spans="1:17" ht="13.8" thickBot="1">
       <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
@@ -1446,23 +1840,24 @@
       <c r="E8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="O8" s="25"/>
-      <c r="P8" s="26"/>
-    </row>
-    <row r="9" spans="1:16" ht="13.5" thickBot="1">
+      <c r="F8" s="154"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="25"/>
+    </row>
+    <row r="9" spans="1:17" ht="13.8" thickBot="1">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
@@ -1475,26 +1870,27 @@
       <c r="D9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="N9" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="O9" s="25"/>
-      <c r="P9" s="26"/>
-    </row>
-    <row r="10" spans="1:16" ht="13.5" thickBot="1">
+      <c r="F9" s="155"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="O9" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="25"/>
+    </row>
+    <row r="10" spans="1:17" ht="13.8" thickBot="1">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
@@ -1507,26 +1903,27 @@
       <c r="D10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="N10" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="O10" s="25"/>
-      <c r="P10" s="26"/>
-    </row>
-    <row r="11" spans="1:16" ht="13.5" thickBot="1">
+      <c r="F10" s="155"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="O10" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="25"/>
+    </row>
+    <row r="11" spans="1:17" ht="13.8" thickBot="1">
       <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
@@ -1539,26 +1936,27 @@
       <c r="D11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="N11" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="O11" s="25"/>
-      <c r="P11" s="26"/>
-    </row>
-    <row r="12" spans="1:16" ht="13.5" thickBot="1">
+      <c r="F11" s="155"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="O11" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="25"/>
+    </row>
+    <row r="12" spans="1:17" ht="13.8" thickBot="1">
       <c r="A12" s="6" t="s">
         <v>13</v>
       </c>
@@ -1574,21 +1972,22 @@
       <c r="E12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="O12" s="25"/>
-      <c r="P12" s="26"/>
-    </row>
-    <row r="13" spans="1:16" ht="13.5" thickBot="1">
+      <c r="F12" s="154"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="25"/>
+    </row>
+    <row r="13" spans="1:17" ht="13.8" thickBot="1">
       <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
@@ -1601,24 +2000,25 @@
       <c r="D13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="O13" s="25"/>
-      <c r="P13" s="26"/>
-    </row>
-    <row r="14" spans="1:16" ht="13.5" thickBot="1">
+      <c r="F13" s="155"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="25"/>
+    </row>
+    <row r="14" spans="1:17" ht="13.8" thickBot="1">
       <c r="A14" s="6" t="s">
         <v>5</v>
       </c>
@@ -1631,26 +2031,27 @@
       <c r="D14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="O14" s="25"/>
-      <c r="P14" s="43" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="13.5" thickBot="1">
+      <c r="F14" s="155"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="13.8" thickBot="1">
       <c r="A15" s="6" t="s">
         <v>6</v>
       </c>
@@ -1663,26 +2064,27 @@
       <c r="D15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="40" t="s">
+      <c r="E15" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="O15" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="P15" s="26"/>
-    </row>
-    <row r="16" spans="1:16" ht="13.5" thickBot="1">
+      <c r="F15" s="155"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="P15" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q15" s="25"/>
+    </row>
+    <row r="16" spans="1:17" ht="13.8" thickBot="1">
       <c r="A16" s="6" t="s">
         <v>7</v>
       </c>
@@ -1695,24 +2097,25 @@
       <c r="D16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="40" t="s">
+      <c r="E16" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="O16" s="25"/>
-      <c r="P16" s="26"/>
-    </row>
-    <row r="17" spans="1:16" ht="13.5" thickBot="1">
+      <c r="F16" s="155"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="25"/>
+    </row>
+    <row r="17" spans="1:17" ht="13.8" thickBot="1">
       <c r="A17" s="6" t="s">
         <v>8</v>
       </c>
@@ -1725,24 +2128,25 @@
       <c r="D17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="40" t="s">
+      <c r="E17" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="O17" s="25"/>
-      <c r="P17" s="26"/>
-    </row>
-    <row r="18" spans="1:16" ht="13.5" thickBot="1">
+      <c r="F17" s="155"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="25"/>
+    </row>
+    <row r="18" spans="1:17" ht="13.8" thickBot="1">
       <c r="A18" s="7" t="s">
         <v>9</v>
       </c>
@@ -1755,246 +2159,252 @@
       <c r="D18" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="41" t="s">
+      <c r="E18" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="M18" s="23"/>
-      <c r="N18" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="O18" s="28"/>
-      <c r="P18" s="29"/>
-    </row>
-    <row r="19" spans="1:16" ht="13.5" thickTop="1"/>
-    <row r="21" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A21" s="31" t="s">
+      <c r="F18" s="156"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="N18" s="22"/>
+      <c r="O18" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="28"/>
+    </row>
+    <row r="19" spans="1:17" ht="13.8" thickTop="1"/>
+    <row r="21" spans="1:17" s="53" customFormat="1" ht="16.2" thickBot="1">
+      <c r="A21" s="52" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A22" s="17" t="s">
+    <row r="22" spans="1:17" s="53" customFormat="1" ht="16.8" thickTop="1" thickBot="1">
+      <c r="A22" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="19" t="s">
+      <c r="F22" s="56"/>
+      <c r="G22" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="H22" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="I22" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="18" t="s">
+      <c r="J22" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="J22" s="18" t="s">
+      <c r="K22" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="K22" s="18" t="s">
+      <c r="L22" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="L22" s="18" t="s">
+      <c r="M22" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="M22" s="20" t="s">
+      <c r="N22" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="N22" s="39" t="s">
+      <c r="O22" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="O22" s="39" t="s">
+      <c r="P22" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="P22" s="39" t="s">
+      <c r="Q22" s="58" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="14.25" thickTop="1" thickBot="1">
-      <c r="A23" s="5" t="s">
+    <row r="23" spans="1:17" s="53" customFormat="1" ht="14.4" thickTop="1" thickBot="1">
+      <c r="A23" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="H23" s="51" t="s">
-        <v>34</v>
-      </c>
-      <c r="I23" s="51"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="21"/>
-      <c r="N23" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="O23" s="37"/>
-      <c r="P23" s="38"/>
-    </row>
-    <row r="24" spans="1:16" ht="13.5" thickBot="1">
-      <c r="A24" s="6" t="s">
+      <c r="E23" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="157"/>
+      <c r="G23" s="62" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" s="63" t="s">
+        <v>34</v>
+      </c>
+      <c r="I23" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="J23" s="64"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="64"/>
+      <c r="M23" s="63"/>
+      <c r="N23" s="65"/>
+      <c r="O23" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="P23" s="67"/>
+      <c r="Q23" s="68"/>
+    </row>
+    <row r="24" spans="1:17" s="53" customFormat="1" ht="13.8" thickBot="1">
+      <c r="A24" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="N24" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="O24" s="25"/>
-      <c r="P24" s="26"/>
-    </row>
-    <row r="25" spans="1:16" ht="13.5" thickBot="1">
-      <c r="A25" s="7" t="s">
+      <c r="E24" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="158"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="74"/>
+      <c r="J24" s="74"/>
+      <c r="K24" s="74"/>
+      <c r="L24" s="74"/>
+      <c r="M24" s="74"/>
+      <c r="N24" s="75" t="s">
+        <v>34</v>
+      </c>
+      <c r="O24" s="76" t="s">
+        <v>34</v>
+      </c>
+      <c r="P24" s="77"/>
+      <c r="Q24" s="78"/>
+    </row>
+    <row r="25" spans="1:17" s="53" customFormat="1" ht="13.8" thickBot="1">
+      <c r="A25" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="M25" s="23"/>
-      <c r="N25" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="O25" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="P25" s="34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="13.5" thickTop="1"/>
-    <row r="28" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A28" s="31" t="s">
+      <c r="F25" s="159"/>
+      <c r="G25" s="82"/>
+      <c r="H25" s="83"/>
+      <c r="I25" s="83"/>
+      <c r="J25" s="83"/>
+      <c r="K25" s="83"/>
+      <c r="L25" s="83"/>
+      <c r="M25" s="83" t="s">
+        <v>34</v>
+      </c>
+      <c r="N25" s="84"/>
+      <c r="O25" s="85" t="s">
+        <v>34</v>
+      </c>
+      <c r="P25" s="86" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q25" s="87" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="13.8" thickTop="1"/>
+    <row r="28" spans="1:17" ht="16.2" thickBot="1">
+      <c r="A28" s="30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A29" s="17" t="s">
+    <row r="29" spans="1:17" ht="16.8" thickTop="1" thickBot="1">
+      <c r="A29" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D29" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="18" t="s">
+      <c r="E29" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F29" s="19" t="s">
+      <c r="F29" s="18"/>
+      <c r="G29" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="G29" s="18" t="s">
+      <c r="H29" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H29" s="18" t="s">
+      <c r="I29" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I29" s="18" t="s">
+      <c r="J29" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="J29" s="18" t="s">
+      <c r="K29" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="K29" s="18" t="s">
+      <c r="L29" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="L29" s="18" t="s">
+      <c r="M29" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="M29" s="20" t="s">
+      <c r="N29" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="N29" s="39" t="s">
+      <c r="O29" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="O29" s="39" t="s">
+      <c r="P29" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="P29" s="39" t="s">
+      <c r="Q29" s="38" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="14.25" thickTop="1" thickBot="1">
-      <c r="A30" s="45" t="s">
+    <row r="30" spans="1:17" ht="14.4" thickTop="1" thickBot="1">
+      <c r="A30" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="48" t="s">
+      <c r="B30" s="47" t="s">
         <v>43</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -2006,63 +2416,65 @@
       <c r="E30" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F30" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="H30" s="51" t="s">
-        <v>34</v>
-      </c>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="51"/>
-      <c r="L30" s="12"/>
-      <c r="M30" s="21"/>
-      <c r="N30" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="O30" s="37"/>
-      <c r="P30" s="38"/>
-    </row>
-    <row r="31" spans="1:16" ht="13.5" thickBot="1">
-      <c r="A31" s="46" t="s">
+      <c r="F30" s="153"/>
+      <c r="G30" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I30" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="J30" s="50"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="20"/>
+      <c r="O30" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="P30" s="36"/>
+      <c r="Q30" s="37"/>
+    </row>
+    <row r="31" spans="1:17" ht="13.8" thickBot="1">
+      <c r="A31" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="29" t="s">
         <v>20</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="F31" s="13"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="N31" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="O31" s="25"/>
-      <c r="P31" s="26"/>
-    </row>
-    <row r="32" spans="1:16" ht="13.5" thickBot="1">
-      <c r="A32" s="44" t="s">
+      <c r="E31" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" s="155"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="O31" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="P31" s="24"/>
+      <c r="Q31" s="25"/>
+    </row>
+    <row r="32" spans="1:17" ht="13.8" thickBot="1">
+      <c r="A32" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="49" t="s">
+      <c r="B32" s="48" t="s">
         <v>45</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -2071,572 +2483,1155 @@
       <c r="D32" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="F32" s="15"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="16"/>
-      <c r="L32" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="M32" s="23"/>
-      <c r="N32" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="O32" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="P32" s="34"/>
-    </row>
-    <row r="33" spans="1:16" ht="13.5" thickTop="1"/>
-    <row r="34" spans="1:16">
-      <c r="A34" s="47" t="s">
+      <c r="E32" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" s="156"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="N32" s="22"/>
+      <c r="O32" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="P32" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q32" s="33"/>
+    </row>
+    <row r="33" spans="1:17" ht="13.8" thickTop="1"/>
+    <row r="34" spans="1:17">
+      <c r="A34" s="46" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A37" s="31" t="s">
+    <row r="37" spans="1:17" s="53" customFormat="1" ht="16.2" thickBot="1">
+      <c r="A37" s="52" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="1" customFormat="1" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A38" s="17" t="s">
+    <row r="38" spans="1:17" s="88" customFormat="1" ht="16.8" thickTop="1" thickBot="1">
+      <c r="A38" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="D38" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="E38" s="18" t="s">
+      <c r="E38" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="F38" s="19" t="s">
+      <c r="F38" s="56"/>
+      <c r="G38" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="G38" s="18" t="s">
+      <c r="H38" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="H38" s="18" t="s">
+      <c r="I38" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="I38" s="18" t="s">
+      <c r="J38" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="J38" s="18" t="s">
+      <c r="K38" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="K38" s="18" t="s">
+      <c r="L38" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="L38" s="18" t="s">
+      <c r="M38" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="M38" s="18" t="s">
+      <c r="N38" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="N38" s="18" t="s">
+      <c r="O38" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="O38" s="18" t="s">
+      <c r="P38" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="P38" s="18" t="s">
+      <c r="Q38" s="55" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A39" s="52" t="s">
+    <row r="39" spans="1:17" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A39" s="89" t="s">
         <v>63</v>
       </c>
-      <c r="B39" s="53" t="s">
+      <c r="B39" s="90" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="53" t="s">
+      <c r="C39" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="D39" s="53" t="s">
+      <c r="D39" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="E39" s="54" t="s">
-        <v>30</v>
-      </c>
-      <c r="F39" s="55"/>
-      <c r="G39" s="56"/>
-      <c r="H39" s="56"/>
-      <c r="I39" s="56"/>
-      <c r="J39" s="56"/>
-      <c r="K39" s="56"/>
-      <c r="L39" s="56"/>
-      <c r="M39" s="57"/>
-      <c r="N39" s="58"/>
-      <c r="O39" s="59"/>
-      <c r="P39" s="60"/>
-    </row>
-    <row r="40" spans="1:16" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A40" s="52" t="s">
+      <c r="E39" s="91" t="s">
+        <v>30</v>
+      </c>
+      <c r="F39" s="160"/>
+      <c r="G39" s="92"/>
+      <c r="H39" s="93"/>
+      <c r="I39" s="93"/>
+      <c r="J39" s="93"/>
+      <c r="K39" s="93"/>
+      <c r="L39" s="93"/>
+      <c r="M39" s="93"/>
+      <c r="N39" s="94"/>
+      <c r="O39" s="95"/>
+      <c r="P39" s="96"/>
+      <c r="Q39" s="97"/>
+    </row>
+    <row r="40" spans="1:17" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A40" s="89" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="53" t="s">
+      <c r="B40" s="90" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="61" t="s">
+      <c r="C40" s="98" t="s">
         <v>79</v>
       </c>
-      <c r="D40" s="61" t="s">
+      <c r="D40" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="E40" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="F40" s="63"/>
-      <c r="G40" s="64"/>
-      <c r="H40" s="64"/>
-      <c r="I40" s="64"/>
-      <c r="J40" s="64"/>
-      <c r="K40" s="64"/>
-      <c r="L40" s="64"/>
-      <c r="M40" s="65"/>
-      <c r="N40" s="66"/>
-      <c r="O40" s="67"/>
-      <c r="P40" s="68" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A41" s="52" t="s">
+      <c r="E40" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="F40" s="161"/>
+      <c r="G40" s="100"/>
+      <c r="H40" s="101"/>
+      <c r="I40" s="101"/>
+      <c r="J40" s="101"/>
+      <c r="K40" s="101"/>
+      <c r="L40" s="101"/>
+      <c r="M40" s="101"/>
+      <c r="N40" s="102"/>
+      <c r="O40" s="103"/>
+      <c r="P40" s="104"/>
+      <c r="Q40" s="105" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A41" s="89" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="53" t="s">
+      <c r="B41" s="90" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="61" t="s">
+      <c r="C41" s="98" t="s">
         <v>80</v>
       </c>
-      <c r="D41" s="61" t="s">
+      <c r="D41" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="E41" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="F41" s="63"/>
-      <c r="G41" s="64"/>
-      <c r="H41" s="64"/>
-      <c r="I41" s="64"/>
-      <c r="J41" s="64"/>
-      <c r="K41" s="64"/>
-      <c r="L41" s="64"/>
-      <c r="M41" s="65"/>
-      <c r="N41" s="66"/>
-      <c r="O41" s="67"/>
-      <c r="P41" s="68"/>
-    </row>
-    <row r="42" spans="1:16" ht="14.25" thickTop="1" thickBot="1">
-      <c r="A42" s="45" t="s">
+      <c r="E41" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="F41" s="161"/>
+      <c r="G41" s="100"/>
+      <c r="H41" s="101"/>
+      <c r="I41" s="101"/>
+      <c r="J41" s="101"/>
+      <c r="K41" s="101"/>
+      <c r="L41" s="101"/>
+      <c r="M41" s="101"/>
+      <c r="N41" s="102"/>
+      <c r="O41" s="103"/>
+      <c r="P41" s="104"/>
+      <c r="Q41" s="105"/>
+    </row>
+    <row r="42" spans="1:17" s="53" customFormat="1" ht="14.4" thickTop="1" thickBot="1">
+      <c r="A42" s="106" t="s">
         <v>64</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="C42" s="30" t="s">
+      <c r="C42" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="E42" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F42" s="13"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="22"/>
-      <c r="N42" s="24"/>
-      <c r="O42" s="25"/>
-      <c r="P42" s="26"/>
-    </row>
-    <row r="43" spans="1:16" ht="14.25" thickTop="1" thickBot="1">
-      <c r="A43" s="45" t="s">
+      <c r="E42" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="F42" s="158"/>
+      <c r="G42" s="73"/>
+      <c r="H42" s="74"/>
+      <c r="I42" s="74"/>
+      <c r="J42" s="74"/>
+      <c r="K42" s="74"/>
+      <c r="L42" s="74"/>
+      <c r="M42" s="74"/>
+      <c r="N42" s="107"/>
+      <c r="O42" s="76"/>
+      <c r="P42" s="77"/>
+      <c r="Q42" s="78"/>
+    </row>
+    <row r="43" spans="1:17" s="53" customFormat="1" ht="14.4" thickTop="1" thickBot="1">
+      <c r="A43" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="30" t="s">
+      <c r="C43" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F43" s="13"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="78" t="s">
-        <v>34</v>
-      </c>
-      <c r="K43" s="78" t="s">
-        <v>34</v>
-      </c>
-      <c r="L43" s="14"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="24"/>
-      <c r="O43" s="25"/>
-      <c r="P43" s="26"/>
-    </row>
-    <row r="44" spans="1:16" ht="14.25" thickTop="1" thickBot="1">
-      <c r="A44" s="45" t="s">
+      <c r="E43" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="F43" s="158"/>
+      <c r="G43" s="73"/>
+      <c r="H43" s="74"/>
+      <c r="I43" s="74"/>
+      <c r="J43" s="74"/>
+      <c r="K43" s="108" t="s">
+        <v>34</v>
+      </c>
+      <c r="L43" s="108" t="s">
+        <v>34</v>
+      </c>
+      <c r="M43" s="74"/>
+      <c r="N43" s="107"/>
+      <c r="O43" s="76"/>
+      <c r="P43" s="77"/>
+      <c r="Q43" s="78"/>
+    </row>
+    <row r="44" spans="1:17" s="53" customFormat="1" ht="14.4" thickTop="1" thickBot="1">
+      <c r="A44" s="106" t="s">
         <v>66</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="30" t="s">
+      <c r="C44" s="71" t="s">
         <v>80</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="E44" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="F44" s="13"/>
-      <c r="G44" s="78" t="s">
-        <v>34</v>
-      </c>
-      <c r="H44" s="78" t="s">
-        <v>34</v>
-      </c>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="22"/>
-      <c r="N44" s="24"/>
-      <c r="O44" s="25"/>
-      <c r="P44" s="26"/>
-    </row>
-    <row r="45" spans="1:16" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A45" s="52" t="s">
+      <c r="E44" s="109" t="s">
+        <v>30</v>
+      </c>
+      <c r="F44" s="162"/>
+      <c r="G44" s="73"/>
+      <c r="H44" s="108" t="s">
+        <v>34</v>
+      </c>
+      <c r="I44" s="108" t="s">
+        <v>34</v>
+      </c>
+      <c r="J44" s="74"/>
+      <c r="K44" s="74"/>
+      <c r="L44" s="74"/>
+      <c r="M44" s="74"/>
+      <c r="N44" s="107"/>
+      <c r="O44" s="76"/>
+      <c r="P44" s="77"/>
+      <c r="Q44" s="78"/>
+    </row>
+    <row r="45" spans="1:17" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A45" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="B45" s="53" t="s">
+      <c r="B45" s="90" t="s">
         <v>76</v>
       </c>
-      <c r="C45" s="61" t="s">
+      <c r="C45" s="98" t="s">
         <v>79</v>
       </c>
-      <c r="D45" s="61" t="s">
+      <c r="D45" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="E45" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="F45" s="63"/>
-      <c r="G45" s="64"/>
-      <c r="H45" s="64"/>
-      <c r="I45" s="64"/>
-      <c r="J45" s="64"/>
-      <c r="K45" s="64"/>
-      <c r="L45" s="64"/>
-      <c r="M45" s="65"/>
-      <c r="N45" s="66"/>
-      <c r="O45" s="67"/>
-      <c r="P45" s="68"/>
-    </row>
-    <row r="46" spans="1:16" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A46" s="52" t="s">
+      <c r="E45" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="F45" s="161"/>
+      <c r="G45" s="100"/>
+      <c r="H45" s="101"/>
+      <c r="I45" s="101"/>
+      <c r="J45" s="101"/>
+      <c r="K45" s="101"/>
+      <c r="L45" s="101"/>
+      <c r="M45" s="101"/>
+      <c r="N45" s="102"/>
+      <c r="O45" s="103"/>
+      <c r="P45" s="104"/>
+      <c r="Q45" s="105"/>
+    </row>
+    <row r="46" spans="1:17" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A46" s="89" t="s">
         <v>68</v>
       </c>
-      <c r="B46" s="53" t="s">
+      <c r="B46" s="90" t="s">
         <v>77</v>
       </c>
-      <c r="C46" s="61" t="s">
+      <c r="C46" s="98" t="s">
         <v>79</v>
       </c>
-      <c r="D46" s="61" t="s">
+      <c r="D46" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="E46" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="F46" s="63"/>
-      <c r="G46" s="64"/>
-      <c r="H46" s="64"/>
-      <c r="I46" s="64"/>
-      <c r="J46" s="64"/>
-      <c r="K46" s="64"/>
-      <c r="L46" s="64"/>
-      <c r="M46" s="65"/>
-      <c r="N46" s="66"/>
-      <c r="O46" s="67" t="s">
-        <v>34</v>
-      </c>
-      <c r="P46" s="68"/>
-    </row>
-    <row r="47" spans="1:16" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A47" s="52" t="s">
+      <c r="E46" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="F46" s="161"/>
+      <c r="G46" s="100"/>
+      <c r="H46" s="101"/>
+      <c r="I46" s="101"/>
+      <c r="J46" s="101"/>
+      <c r="K46" s="101"/>
+      <c r="L46" s="101"/>
+      <c r="M46" s="101"/>
+      <c r="N46" s="102"/>
+      <c r="O46" s="103"/>
+      <c r="P46" s="104" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q46" s="105"/>
+    </row>
+    <row r="47" spans="1:17" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A47" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="53" t="s">
+      <c r="B47" s="90" t="s">
         <v>78</v>
       </c>
-      <c r="C47" s="61" t="s">
+      <c r="C47" s="98" t="s">
         <v>80</v>
       </c>
-      <c r="D47" s="61" t="s">
+      <c r="D47" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="E47" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="F47" s="63" t="s">
-        <v>34</v>
-      </c>
-      <c r="G47" s="64"/>
-      <c r="H47" s="64"/>
-      <c r="I47" s="64" t="s">
-        <v>34</v>
-      </c>
-      <c r="J47" s="64"/>
-      <c r="K47" s="64"/>
-      <c r="L47" s="64"/>
-      <c r="M47" s="65"/>
-      <c r="N47" s="66"/>
-      <c r="O47" s="67"/>
-      <c r="P47" s="68"/>
-    </row>
-    <row r="48" spans="1:16" ht="14.25" thickTop="1" thickBot="1">
-      <c r="A48" s="45" t="s">
+      <c r="E47" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="F47" s="161"/>
+      <c r="G47" s="100" t="s">
+        <v>34</v>
+      </c>
+      <c r="H47" s="101"/>
+      <c r="I47" s="101"/>
+      <c r="J47" s="101" t="s">
+        <v>34</v>
+      </c>
+      <c r="K47" s="101"/>
+      <c r="L47" s="101"/>
+      <c r="M47" s="101"/>
+      <c r="N47" s="102"/>
+      <c r="O47" s="103"/>
+      <c r="P47" s="104"/>
+      <c r="Q47" s="105"/>
+    </row>
+    <row r="48" spans="1:17" s="53" customFormat="1" ht="14.4" thickTop="1" thickBot="1">
+      <c r="A48" s="106" t="s">
         <v>70</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="C48" s="30" t="s">
+      <c r="C48" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="E48" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="F48" s="13"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="32" t="s">
+      <c r="E48" s="109" t="s">
+        <v>30</v>
+      </c>
+      <c r="F48" s="162"/>
+      <c r="G48" s="73"/>
+      <c r="H48" s="74"/>
+      <c r="I48" s="74"/>
+      <c r="J48" s="74"/>
+      <c r="K48" s="74"/>
+      <c r="L48" s="74"/>
+      <c r="M48" s="74"/>
+      <c r="N48" s="75" t="s">
         <v>83</v>
       </c>
-      <c r="N48" s="24"/>
-      <c r="O48" s="25"/>
-      <c r="P48" s="26"/>
-    </row>
-    <row r="49" spans="1:16" ht="14.25" thickTop="1" thickBot="1">
-      <c r="A49" s="45" t="s">
+      <c r="O48" s="76"/>
+      <c r="P48" s="77"/>
+      <c r="Q48" s="78"/>
+    </row>
+    <row r="49" spans="1:19" s="53" customFormat="1" ht="14.4" thickTop="1" thickBot="1">
+      <c r="A49" s="106" t="s">
         <v>71</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="C49" s="30" t="s">
+      <c r="C49" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="E49" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="F49" s="13"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
-      <c r="L49" s="14"/>
-      <c r="M49" s="22"/>
-      <c r="N49" s="24"/>
-      <c r="O49" s="25"/>
-      <c r="P49" s="43"/>
-    </row>
-    <row r="50" spans="1:16" ht="14.25" thickTop="1" thickBot="1">
-      <c r="A50" s="45" t="s">
+      <c r="E49" s="109" t="s">
+        <v>30</v>
+      </c>
+      <c r="F49" s="162"/>
+      <c r="G49" s="73"/>
+      <c r="H49" s="74"/>
+      <c r="I49" s="74"/>
+      <c r="J49" s="74"/>
+      <c r="K49" s="74"/>
+      <c r="L49" s="74"/>
+      <c r="M49" s="74"/>
+      <c r="N49" s="107"/>
+      <c r="O49" s="76"/>
+      <c r="P49" s="77"/>
+      <c r="Q49" s="110"/>
+    </row>
+    <row r="50" spans="1:19" s="53" customFormat="1" ht="14.4" thickTop="1" thickBot="1">
+      <c r="A50" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="C50" s="30" t="s">
+      <c r="C50" s="71" t="s">
         <v>80</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="E50" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="F50" s="13"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-      <c r="L50" s="14"/>
-      <c r="M50" s="22"/>
-      <c r="N50" s="24"/>
-      <c r="O50" s="42"/>
-      <c r="P50" s="26"/>
-    </row>
-    <row r="51" spans="1:16" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A51" s="52" t="s">
+      <c r="E50" s="109" t="s">
+        <v>30</v>
+      </c>
+      <c r="F50" s="162"/>
+      <c r="G50" s="73"/>
+      <c r="H50" s="74"/>
+      <c r="I50" s="74"/>
+      <c r="J50" s="74"/>
+      <c r="K50" s="74"/>
+      <c r="L50" s="74"/>
+      <c r="M50" s="74"/>
+      <c r="N50" s="107"/>
+      <c r="O50" s="76"/>
+      <c r="P50" s="111"/>
+      <c r="Q50" s="78"/>
+    </row>
+    <row r="51" spans="1:19" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A51" s="89" t="s">
         <v>73</v>
       </c>
-      <c r="B51" s="53" t="s">
+      <c r="B51" s="90" t="s">
         <v>76</v>
       </c>
-      <c r="C51" s="61" t="s">
+      <c r="C51" s="98" t="s">
         <v>79</v>
       </c>
-      <c r="D51" s="61" t="s">
+      <c r="D51" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="E51" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="F51" s="63"/>
-      <c r="G51" s="64"/>
-      <c r="H51" s="64"/>
-      <c r="I51" s="64"/>
-      <c r="J51" s="64"/>
-      <c r="K51" s="64"/>
-      <c r="L51" s="64"/>
-      <c r="M51" s="65" t="s">
+      <c r="E51" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="F51" s="161"/>
+      <c r="G51" s="100"/>
+      <c r="H51" s="101"/>
+      <c r="I51" s="101"/>
+      <c r="J51" s="101"/>
+      <c r="K51" s="101"/>
+      <c r="L51" s="101"/>
+      <c r="M51" s="101"/>
+      <c r="N51" s="102" t="s">
         <v>82</v>
       </c>
-      <c r="N51" s="66"/>
-      <c r="O51" s="67"/>
-      <c r="P51" s="68"/>
-    </row>
-    <row r="52" spans="1:16" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A52" s="52" t="s">
+      <c r="O51" s="103"/>
+      <c r="P51" s="104"/>
+      <c r="Q51" s="105"/>
+    </row>
+    <row r="52" spans="1:19" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A52" s="89" t="s">
         <v>74</v>
       </c>
-      <c r="B52" s="53" t="s">
+      <c r="B52" s="90" t="s">
         <v>77</v>
       </c>
-      <c r="C52" s="61" t="s">
+      <c r="C52" s="98" t="s">
         <v>79</v>
       </c>
-      <c r="D52" s="61" t="s">
+      <c r="D52" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="E52" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="F52" s="63"/>
-      <c r="G52" s="64"/>
-      <c r="H52" s="64"/>
-      <c r="I52" s="64"/>
-      <c r="J52" s="64"/>
-      <c r="K52" s="64"/>
-      <c r="L52" s="64"/>
-      <c r="M52" s="65"/>
-      <c r="N52" s="66"/>
-      <c r="O52" s="67"/>
-      <c r="P52" s="68"/>
-    </row>
-    <row r="53" spans="1:16" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A53" s="52" t="s">
+      <c r="E52" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="F52" s="161"/>
+      <c r="G52" s="100"/>
+      <c r="H52" s="101"/>
+      <c r="I52" s="101"/>
+      <c r="J52" s="101"/>
+      <c r="K52" s="101"/>
+      <c r="L52" s="101"/>
+      <c r="M52" s="101"/>
+      <c r="N52" s="102"/>
+      <c r="O52" s="103"/>
+      <c r="P52" s="104"/>
+      <c r="Q52" s="105"/>
+    </row>
+    <row r="53" spans="1:19" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A53" s="89" t="s">
         <v>75</v>
       </c>
-      <c r="B53" s="53" t="s">
+      <c r="B53" s="90" t="s">
         <v>78</v>
       </c>
-      <c r="C53" s="69" t="s">
+      <c r="C53" s="112" t="s">
         <v>80</v>
       </c>
-      <c r="D53" s="69" t="s">
+      <c r="D53" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="E53" s="70" t="s">
-        <v>30</v>
-      </c>
-      <c r="F53" s="71"/>
-      <c r="G53" s="72"/>
-      <c r="H53" s="72"/>
-      <c r="I53" s="72"/>
-      <c r="J53" s="72"/>
-      <c r="K53" s="72"/>
-      <c r="L53" s="72"/>
-      <c r="M53" s="73"/>
-      <c r="N53" s="74"/>
-      <c r="O53" s="75"/>
-      <c r="P53" s="76"/>
-    </row>
-    <row r="54" spans="1:16" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A54" s="52" t="s">
+      <c r="E53" s="113" t="s">
+        <v>30</v>
+      </c>
+      <c r="F53" s="163"/>
+      <c r="G53" s="114"/>
+      <c r="H53" s="115"/>
+      <c r="I53" s="115"/>
+      <c r="J53" s="115"/>
+      <c r="K53" s="115"/>
+      <c r="L53" s="115"/>
+      <c r="M53" s="115"/>
+      <c r="N53" s="116"/>
+      <c r="O53" s="117"/>
+      <c r="P53" s="118"/>
+      <c r="Q53" s="119"/>
+    </row>
+    <row r="54" spans="1:19" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A54" s="89" t="s">
         <v>84</v>
       </c>
-      <c r="B54" s="53" t="s">
+      <c r="B54" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="C54" s="61" t="s">
+      <c r="C54" s="98" t="s">
         <v>79</v>
       </c>
-      <c r="D54" s="61" t="s">
+      <c r="D54" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="E54" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="F54" s="63"/>
-      <c r="G54" s="64"/>
-      <c r="H54" s="64"/>
-      <c r="I54" s="64"/>
-      <c r="J54" s="64"/>
-      <c r="K54" s="64"/>
-      <c r="L54" s="64" t="s">
-        <v>34</v>
-      </c>
-      <c r="M54" s="65"/>
-      <c r="N54" s="66"/>
-      <c r="O54" s="67"/>
-      <c r="P54" s="68"/>
-    </row>
-    <row r="56" spans="1:16">
-      <c r="A56" t="s">
+      <c r="E54" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="F54" s="161"/>
+      <c r="G54" s="100"/>
+      <c r="H54" s="101"/>
+      <c r="I54" s="101"/>
+      <c r="J54" s="101"/>
+      <c r="K54" s="101"/>
+      <c r="L54" s="101"/>
+      <c r="M54" s="101" t="s">
+        <v>34</v>
+      </c>
+      <c r="N54" s="102"/>
+      <c r="O54" s="103"/>
+      <c r="P54" s="104"/>
+      <c r="Q54" s="105"/>
+    </row>
+    <row r="55" spans="1:19" s="53" customFormat="1"/>
+    <row r="56" spans="1:19" s="53" customFormat="1">
+      <c r="A56" s="53" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="57" spans="1:16">
-      <c r="A57" s="77" t="s">
+      <c r="B56" s="53" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" s="53" customFormat="1">
+      <c r="A57" s="120" t="s">
         <v>85</v>
       </c>
+      <c r="B57" s="53" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" s="122" customFormat="1" ht="16.2" thickBot="1">
+      <c r="A60" s="121" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" ht="16.8" thickTop="1" thickBot="1">
+      <c r="A61" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E61" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F61" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="G61" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H61" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I61" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J61" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="K61" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="L61" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="M61" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="N61" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="O61" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="P61" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q61" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="R61" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="S61" s="38" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A62" s="174" t="s">
+        <v>111</v>
+      </c>
+      <c r="B62" s="151" t="s">
+        <v>88</v>
+      </c>
+      <c r="C62" s="123" t="s">
+        <v>79</v>
+      </c>
+      <c r="D62" s="175" t="s">
+        <v>120</v>
+      </c>
+      <c r="E62" s="124" t="s">
+        <v>30</v>
+      </c>
+      <c r="F62" s="175" t="s">
+        <v>121</v>
+      </c>
+      <c r="G62" s="125"/>
+      <c r="H62" s="126"/>
+      <c r="I62" s="126"/>
+      <c r="J62" s="126"/>
+      <c r="K62" s="126"/>
+      <c r="L62" s="126"/>
+      <c r="M62" s="152" t="s">
+        <v>34</v>
+      </c>
+      <c r="N62" s="127"/>
+      <c r="O62" s="167" t="s">
+        <v>34</v>
+      </c>
+      <c r="P62" s="128"/>
+      <c r="Q62" s="129"/>
+      <c r="R62" s="129"/>
+      <c r="S62" s="129"/>
+    </row>
+    <row r="63" spans="1:19" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A63" s="174" t="s">
+        <v>112</v>
+      </c>
+      <c r="B63" s="151" t="s">
+        <v>88</v>
+      </c>
+      <c r="C63" s="130" t="s">
+        <v>79</v>
+      </c>
+      <c r="D63" s="175" t="s">
+        <v>120</v>
+      </c>
+      <c r="E63" s="131" t="s">
+        <v>30</v>
+      </c>
+      <c r="F63" s="164" t="s">
+        <v>94</v>
+      </c>
+      <c r="G63" s="132"/>
+      <c r="H63" s="133"/>
+      <c r="I63" s="133"/>
+      <c r="J63" s="133"/>
+      <c r="K63" s="133"/>
+      <c r="L63" s="133"/>
+      <c r="M63" s="133"/>
+      <c r="N63" s="165" t="s">
+        <v>82</v>
+      </c>
+      <c r="O63" s="168" t="s">
+        <v>34</v>
+      </c>
+      <c r="P63" s="135"/>
+      <c r="Q63" s="136"/>
+      <c r="R63" s="136"/>
+      <c r="S63" s="136"/>
+    </row>
+    <row r="64" spans="1:19" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A64" s="150" t="s">
+        <v>87</v>
+      </c>
+      <c r="B64" s="151" t="s">
+        <v>88</v>
+      </c>
+      <c r="C64" s="164" t="s">
+        <v>79</v>
+      </c>
+      <c r="D64" s="175" t="s">
+        <v>120</v>
+      </c>
+      <c r="E64" s="131" t="s">
+        <v>30</v>
+      </c>
+      <c r="F64" s="164" t="s">
+        <v>96</v>
+      </c>
+      <c r="G64" s="132"/>
+      <c r="H64" s="133"/>
+      <c r="I64" s="133"/>
+      <c r="J64" s="133"/>
+      <c r="K64" s="133"/>
+      <c r="L64" s="133"/>
+      <c r="M64" s="133"/>
+      <c r="N64" s="165" t="s">
+        <v>83</v>
+      </c>
+      <c r="O64" s="168" t="s">
+        <v>34</v>
+      </c>
+      <c r="P64" s="135"/>
+      <c r="Q64" s="136"/>
+      <c r="R64" s="136"/>
+      <c r="S64" s="136"/>
+    </row>
+    <row r="65" spans="1:19" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A65" s="174" t="s">
+        <v>113</v>
+      </c>
+      <c r="B65" s="151" t="s">
+        <v>88</v>
+      </c>
+      <c r="C65" s="137" t="s">
+        <v>79</v>
+      </c>
+      <c r="D65" s="175" t="s">
+        <v>120</v>
+      </c>
+      <c r="E65" s="146" t="s">
+        <v>30</v>
+      </c>
+      <c r="F65" s="164" t="s">
+        <v>99</v>
+      </c>
+      <c r="G65" s="139"/>
+      <c r="H65" s="140"/>
+      <c r="I65" s="140"/>
+      <c r="J65" s="140"/>
+      <c r="K65" s="140"/>
+      <c r="L65" s="140"/>
+      <c r="M65" s="140"/>
+      <c r="N65" s="141"/>
+      <c r="O65" s="167" t="s">
+        <v>34</v>
+      </c>
+      <c r="P65" s="143"/>
+      <c r="Q65" s="148"/>
+      <c r="R65" s="148" t="s">
+        <v>34</v>
+      </c>
+      <c r="S65" s="148"/>
+    </row>
+    <row r="66" spans="1:19" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A66" s="174" t="s">
+        <v>110</v>
+      </c>
+      <c r="B66" s="151" t="s">
+        <v>77</v>
+      </c>
+      <c r="C66" s="137" t="s">
+        <v>79</v>
+      </c>
+      <c r="D66" s="175" t="s">
+        <v>120</v>
+      </c>
+      <c r="E66" s="138" t="s">
+        <v>30</v>
+      </c>
+      <c r="F66" s="164" t="s">
+        <v>97</v>
+      </c>
+      <c r="G66" s="139"/>
+      <c r="H66" s="140"/>
+      <c r="I66" s="140"/>
+      <c r="J66" s="140"/>
+      <c r="K66" s="140"/>
+      <c r="L66" s="140"/>
+      <c r="M66" s="140"/>
+      <c r="N66" s="141"/>
+      <c r="O66" s="167" t="s">
+        <v>34</v>
+      </c>
+      <c r="P66" s="143" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q66" s="144"/>
+      <c r="R66" s="144"/>
+      <c r="S66" s="144"/>
+    </row>
+    <row r="67" spans="1:19" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A67" s="174" t="s">
+        <v>109</v>
+      </c>
+      <c r="B67" s="151" t="s">
+        <v>88</v>
+      </c>
+      <c r="C67" s="137" t="s">
+        <v>80</v>
+      </c>
+      <c r="D67" s="175" t="s">
+        <v>120</v>
+      </c>
+      <c r="E67" s="138" t="s">
+        <v>30</v>
+      </c>
+      <c r="F67" s="164" t="s">
+        <v>97</v>
+      </c>
+      <c r="G67" s="139" t="s">
+        <v>34</v>
+      </c>
+      <c r="H67" s="140"/>
+      <c r="I67" s="140"/>
+      <c r="J67" s="140"/>
+      <c r="K67" s="145"/>
+      <c r="L67" s="145"/>
+      <c r="M67" s="140"/>
+      <c r="N67" s="141"/>
+      <c r="O67" s="167" t="s">
+        <v>34</v>
+      </c>
+      <c r="P67" s="143"/>
+      <c r="Q67" s="144"/>
+      <c r="R67" s="144"/>
+      <c r="S67" s="144"/>
+    </row>
+    <row r="68" spans="1:19" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A68" s="174" t="s">
+        <v>114</v>
+      </c>
+      <c r="B68" s="151" t="s">
+        <v>88</v>
+      </c>
+      <c r="C68" s="164" t="s">
+        <v>80</v>
+      </c>
+      <c r="D68" s="175" t="s">
+        <v>120</v>
+      </c>
+      <c r="E68" s="131" t="s">
+        <v>30</v>
+      </c>
+      <c r="F68" s="164" t="s">
+        <v>97</v>
+      </c>
+      <c r="G68" s="132"/>
+      <c r="H68" s="133"/>
+      <c r="I68" s="133"/>
+      <c r="J68" s="166" t="s">
+        <v>34</v>
+      </c>
+      <c r="K68" s="133"/>
+      <c r="L68" s="133"/>
+      <c r="M68" s="133"/>
+      <c r="N68" s="134"/>
+      <c r="O68" s="167" t="s">
+        <v>34</v>
+      </c>
+      <c r="P68" s="135"/>
+      <c r="Q68" s="136"/>
+      <c r="R68" s="136"/>
+      <c r="S68" s="136"/>
+    </row>
+    <row r="69" spans="1:19" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A69" s="174" t="s">
+        <v>115</v>
+      </c>
+      <c r="B69" s="151" t="s">
+        <v>77</v>
+      </c>
+      <c r="C69" s="137" t="s">
+        <v>79</v>
+      </c>
+      <c r="D69" s="175" t="s">
+        <v>120</v>
+      </c>
+      <c r="E69" s="146" t="s">
+        <v>30</v>
+      </c>
+      <c r="F69" s="164" t="s">
+        <v>98</v>
+      </c>
+      <c r="G69" s="139"/>
+      <c r="H69" s="140"/>
+      <c r="I69" s="140"/>
+      <c r="J69" s="140"/>
+      <c r="K69" s="140"/>
+      <c r="L69" s="140" t="s">
+        <v>34</v>
+      </c>
+      <c r="M69" s="140"/>
+      <c r="N69" s="147"/>
+      <c r="O69" s="167" t="s">
+        <v>34</v>
+      </c>
+      <c r="P69" s="143"/>
+      <c r="Q69" s="144"/>
+      <c r="R69" s="144"/>
+      <c r="S69" s="144"/>
+    </row>
+    <row r="70" spans="1:19" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A70" s="174" t="s">
+        <v>116</v>
+      </c>
+      <c r="B70" s="151" t="s">
+        <v>77</v>
+      </c>
+      <c r="C70" s="164" t="s">
+        <v>79</v>
+      </c>
+      <c r="D70" s="175" t="s">
+        <v>120</v>
+      </c>
+      <c r="E70" s="131" t="s">
+        <v>30</v>
+      </c>
+      <c r="F70" s="164" t="s">
+        <v>98</v>
+      </c>
+      <c r="G70" s="132"/>
+      <c r="H70" s="133"/>
+      <c r="I70" s="133"/>
+      <c r="J70" s="133"/>
+      <c r="K70" s="166" t="s">
+        <v>34</v>
+      </c>
+      <c r="L70" s="133"/>
+      <c r="M70" s="133"/>
+      <c r="N70" s="134"/>
+      <c r="O70" s="167" t="s">
+        <v>34</v>
+      </c>
+      <c r="P70" s="135"/>
+      <c r="Q70" s="136"/>
+      <c r="R70" s="136"/>
+      <c r="S70" s="136"/>
+    </row>
+    <row r="71" spans="1:19" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A71" s="174" t="s">
+        <v>117</v>
+      </c>
+      <c r="B71" s="151" t="s">
+        <v>88</v>
+      </c>
+      <c r="C71" s="137" t="s">
+        <v>80</v>
+      </c>
+      <c r="D71" s="175" t="s">
+        <v>120</v>
+      </c>
+      <c r="E71" s="146" t="s">
+        <v>30</v>
+      </c>
+      <c r="F71" s="164" t="s">
+        <v>98</v>
+      </c>
+      <c r="G71" s="139"/>
+      <c r="H71" s="145" t="s">
+        <v>34</v>
+      </c>
+      <c r="I71" s="145"/>
+      <c r="J71" s="140"/>
+      <c r="K71" s="140"/>
+      <c r="L71" s="140"/>
+      <c r="M71" s="140"/>
+      <c r="N71" s="141"/>
+      <c r="O71" s="167" t="s">
+        <v>34</v>
+      </c>
+      <c r="P71" s="143"/>
+      <c r="Q71" s="144"/>
+      <c r="R71" s="144"/>
+      <c r="S71" s="144"/>
+    </row>
+    <row r="72" spans="1:19" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A72" s="174" t="s">
+        <v>118</v>
+      </c>
+      <c r="B72" s="151" t="s">
+        <v>88</v>
+      </c>
+      <c r="C72" s="164" t="s">
+        <v>80</v>
+      </c>
+      <c r="D72" s="175" t="s">
+        <v>120</v>
+      </c>
+      <c r="E72" s="131" t="s">
+        <v>30</v>
+      </c>
+      <c r="F72" s="164" t="s">
+        <v>98</v>
+      </c>
+      <c r="G72" s="132"/>
+      <c r="H72" s="133"/>
+      <c r="I72" s="166" t="s">
+        <v>34</v>
+      </c>
+      <c r="J72" s="133"/>
+      <c r="K72" s="133"/>
+      <c r="L72" s="133"/>
+      <c r="M72" s="133"/>
+      <c r="N72" s="134"/>
+      <c r="O72" s="167" t="s">
+        <v>34</v>
+      </c>
+      <c r="P72" s="135"/>
+      <c r="Q72" s="136"/>
+      <c r="R72" s="136"/>
+      <c r="S72" s="136"/>
+    </row>
+    <row r="73" spans="1:19" s="53" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A73" s="174" t="s">
+        <v>119</v>
+      </c>
+      <c r="B73" s="151" t="s">
+        <v>88</v>
+      </c>
+      <c r="C73" s="137" t="s">
+        <v>79</v>
+      </c>
+      <c r="D73" s="175" t="s">
+        <v>120</v>
+      </c>
+      <c r="E73" s="146" t="s">
+        <v>30</v>
+      </c>
+      <c r="F73" s="164" t="s">
+        <v>95</v>
+      </c>
+      <c r="G73" s="139"/>
+      <c r="H73" s="140"/>
+      <c r="I73" s="140"/>
+      <c r="J73" s="140"/>
+      <c r="K73" s="140"/>
+      <c r="L73" s="140"/>
+      <c r="M73" s="140"/>
+      <c r="N73" s="141"/>
+      <c r="O73" s="142"/>
+      <c r="P73" s="149"/>
+      <c r="Q73" s="144"/>
+      <c r="R73" s="144"/>
+      <c r="S73" s="144" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" ht="13.8" thickBot="1"/>
+    <row r="76" spans="1:19" s="169" customFormat="1" ht="14.4" thickTop="1" thickBot="1">
+      <c r="A76" s="172" t="s">
+        <v>89</v>
+      </c>
+      <c r="B76" s="173" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" ht="15" thickTop="1">
+      <c r="A77" s="170">
+        <v>1</v>
+      </c>
+      <c r="B77" s="171" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19">
+      <c r="A78" s="13">
+        <v>2</v>
+      </c>
+      <c r="B78" s="51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19">
+      <c r="A79" s="13">
+        <v>3</v>
+      </c>
+      <c r="B79" s="51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19">
+      <c r="A80" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="B80" s="51" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="B81" s="51" t="s">
+        <v>105</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <sortState ref="A62:S73">
+    <sortCondition ref="F62:F73"/>
+  </sortState>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="93" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="41" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -2649,38 +3644,38 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="54.28515625" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" customWidth="1"/>
+    <col min="4" max="4" width="54.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:4" ht="16.2" thickBot="1">
+      <c r="A1" s="30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:4" ht="16.8" thickTop="1" thickBot="1">
+      <c r="A2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.25" thickTop="1" thickBot="1">
-      <c r="A3" s="45" t="s">
+    <row r="3" spans="1:4" ht="14.4" thickTop="1" thickBot="1">
+      <c r="A3" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="47" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2691,7 +3686,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated deployed_service with most recent training grid changes.
</commit_message>
<xml_diff>
--- a/Documentation/management/osu/deployed_services.xlsx
+++ b/Documentation/management/osu/deployed_services.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="72" windowWidth="19992" windowHeight="14616"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="19995" windowHeight="14610"/>
   </bookViews>
   <sheets>
     <sheet name="services" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="125">
   <si>
     <t>cagrid01.bmi.ohio-state.edu:8080</t>
   </si>
@@ -302,9 +302,6 @@
     <t>trainingvm01.bmi.ohio-state.edu</t>
   </si>
   <si>
-    <t>trainingvm07.bmi.ohio-state.edu</t>
-  </si>
-  <si>
     <t>trainingvm02.bmi.ohio-state.edu</t>
   </si>
   <si>
@@ -387,16 +384,29 @@
   </si>
   <si>
     <t>portal</t>
+  </si>
+  <si>
+    <t>portal.training.cagrid.org now points to http://cagrid-portal.semanticbits.com/</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -477,7 +487,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -513,8 +523,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="35">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -994,15 +1010,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1035,12 +1071,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1060,15 +1096,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1077,66 +1113,66 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="29" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="26" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="27" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="23" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="24" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="26" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="27" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="28" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="14" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="23" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="24" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1152,112 +1188,112 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="30" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="26" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="27" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="27" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="28" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="20" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="23" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="23" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="24" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="30" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="26" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="27" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="27" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="28" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="20" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="23" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="23" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="24" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1275,36 +1311,34 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="31" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="17" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="21" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="25" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="25" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="22" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="31" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="17" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="21" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="25" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="25" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="22" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1316,7 +1350,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1345,12 +1379,32 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -1653,36 +1707,36 @@
   <dimension ref="A2:S81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+      <selection activeCell="A74" sqref="A74:B74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="54.5546875" customWidth="1"/>
+    <col min="1" max="1" width="54.5703125" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="6.109375" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" customWidth="1"/>
-    <col min="6" max="6" width="29.109375" customWidth="1"/>
-    <col min="7" max="7" width="6.5546875" customWidth="1"/>
-    <col min="8" max="8" width="6.109375" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="4.88671875" customWidth="1"/>
-    <col min="11" max="11" width="5.44140625" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" customWidth="1"/>
-    <col min="13" max="13" width="7.44140625" customWidth="1"/>
-    <col min="14" max="14" width="5.33203125" customWidth="1"/>
-    <col min="15" max="15" width="9.5546875" customWidth="1"/>
-    <col min="16" max="16" width="13.88671875" customWidth="1"/>
-    <col min="17" max="17" width="9.5546875" customWidth="1"/>
+    <col min="10" max="10" width="4.85546875" customWidth="1"/>
+    <col min="11" max="11" width="5.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" customWidth="1"/>
+    <col min="14" max="14" width="5.28515625" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="16.2" thickBot="1">
+    <row r="2" spans="1:17" ht="16.5" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" ht="16.8" thickTop="1" thickBot="1">
+    <row r="3" spans="1:17" s="1" customFormat="1" ht="17.25" thickTop="1" thickBot="1">
       <c r="A3" s="16" t="s">
         <v>15</v>
       </c>
@@ -1733,7 +1787,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="14.4" thickTop="1" thickBot="1">
+    <row r="4" spans="1:17" ht="14.25" thickTop="1" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1768,7 +1822,7 @@
       <c r="P4" s="36"/>
       <c r="Q4" s="37"/>
     </row>
-    <row r="5" spans="1:17" ht="13.8" thickBot="1">
+    <row r="5" spans="1:17" ht="13.5" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1801,7 +1855,7 @@
       <c r="P5" s="24"/>
       <c r="Q5" s="25"/>
     </row>
-    <row r="6" spans="1:17" ht="13.8" thickBot="1">
+    <row r="6" spans="1:17" ht="13.5" thickBot="1">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1832,7 +1886,7 @@
       <c r="P6" s="24"/>
       <c r="Q6" s="25"/>
     </row>
-    <row r="7" spans="1:17" ht="13.8" thickBot="1">
+    <row r="7" spans="1:17" ht="13.5" thickBot="1">
       <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
@@ -1863,7 +1917,7 @@
       <c r="P7" s="24"/>
       <c r="Q7" s="25"/>
     </row>
-    <row r="8" spans="1:17" ht="13.8" thickBot="1">
+    <row r="8" spans="1:17" ht="13.5" thickBot="1">
       <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
@@ -1896,7 +1950,7 @@
       <c r="P8" s="24"/>
       <c r="Q8" s="25"/>
     </row>
-    <row r="9" spans="1:17" ht="13.8" thickBot="1">
+    <row r="9" spans="1:17" ht="13.5" thickBot="1">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
@@ -1929,7 +1983,7 @@
       <c r="P9" s="24"/>
       <c r="Q9" s="25"/>
     </row>
-    <row r="10" spans="1:17" ht="13.8" thickBot="1">
+    <row r="10" spans="1:17" ht="13.5" thickBot="1">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
@@ -1962,7 +2016,7 @@
       <c r="P10" s="24"/>
       <c r="Q10" s="25"/>
     </row>
-    <row r="11" spans="1:17" ht="13.8" thickBot="1">
+    <row r="11" spans="1:17" ht="13.5" thickBot="1">
       <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
@@ -1995,7 +2049,7 @@
       <c r="P11" s="24"/>
       <c r="Q11" s="25"/>
     </row>
-    <row r="12" spans="1:17" ht="13.8" thickBot="1">
+    <row r="12" spans="1:17" ht="13.5" thickBot="1">
       <c r="A12" s="6" t="s">
         <v>13</v>
       </c>
@@ -2026,7 +2080,7 @@
       <c r="P12" s="24"/>
       <c r="Q12" s="25"/>
     </row>
-    <row r="13" spans="1:17" ht="13.8" thickBot="1">
+    <row r="13" spans="1:17" ht="13.5" thickBot="1">
       <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
@@ -2057,7 +2111,7 @@
       <c r="P13" s="24"/>
       <c r="Q13" s="25"/>
     </row>
-    <row r="14" spans="1:17" ht="13.8" thickBot="1">
+    <row r="14" spans="1:17" ht="13.5" thickBot="1">
       <c r="A14" s="6" t="s">
         <v>5</v>
       </c>
@@ -2090,7 +2144,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="13.8" thickBot="1">
+    <row r="15" spans="1:17" ht="13.5" thickBot="1">
       <c r="A15" s="6" t="s">
         <v>6</v>
       </c>
@@ -2123,7 +2177,7 @@
       </c>
       <c r="Q15" s="25"/>
     </row>
-    <row r="16" spans="1:17" ht="13.8" thickBot="1">
+    <row r="16" spans="1:17" ht="13.5" thickBot="1">
       <c r="A16" s="6" t="s">
         <v>7</v>
       </c>
@@ -2154,7 +2208,7 @@
       <c r="P16" s="24"/>
       <c r="Q16" s="25"/>
     </row>
-    <row r="17" spans="1:17" ht="13.8" thickBot="1">
+    <row r="17" spans="1:17" ht="13.5" thickBot="1">
       <c r="A17" s="6" t="s">
         <v>8</v>
       </c>
@@ -2185,7 +2239,7 @@
       <c r="P17" s="24"/>
       <c r="Q17" s="25"/>
     </row>
-    <row r="18" spans="1:17" ht="13.8" thickBot="1">
+    <row r="18" spans="1:17" ht="13.5" thickBot="1">
       <c r="A18" s="7" t="s">
         <v>9</v>
       </c>
@@ -2218,13 +2272,13 @@
       <c r="P18" s="27"/>
       <c r="Q18" s="28"/>
     </row>
-    <row r="19" spans="1:17" ht="13.8" thickTop="1"/>
-    <row r="21" spans="1:17" s="104" customFormat="1" ht="16.2" thickBot="1">
+    <row r="19" spans="1:17" ht="13.5" thickTop="1"/>
+    <row r="21" spans="1:17" s="104" customFormat="1" ht="16.5" thickBot="1">
       <c r="A21" s="103" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="104" customFormat="1" ht="16.8" thickTop="1" thickBot="1">
+    <row r="22" spans="1:17" s="104" customFormat="1" ht="17.25" thickTop="1" thickBot="1">
       <c r="A22" s="105" t="s">
         <v>15</v>
       </c>
@@ -2262,21 +2316,21 @@
       <c r="M22" s="106" t="s">
         <v>24</v>
       </c>
-      <c r="N22" s="156" t="s">
+      <c r="N22" s="154" t="s">
         <v>25</v>
       </c>
-      <c r="O22" s="157" t="s">
+      <c r="O22" s="155" t="s">
         <v>26</v>
       </c>
-      <c r="P22" s="157" t="s">
+      <c r="P22" s="155" t="s">
         <v>38</v>
       </c>
-      <c r="Q22" s="157" t="s">
+      <c r="Q22" s="155" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="104" customFormat="1" ht="14.4" thickTop="1" thickBot="1">
-      <c r="A23" s="158" t="s">
+    <row r="23" spans="1:17" s="104" customFormat="1" ht="14.25" thickTop="1" thickBot="1">
+      <c r="A23" s="156" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="129" t="s">
@@ -2288,32 +2342,32 @@
       <c r="D23" s="129" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="159" t="s">
+      <c r="E23" s="157" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="160"/>
-      <c r="G23" s="161" t="s">
-        <v>34</v>
-      </c>
-      <c r="H23" s="162" t="s">
-        <v>34</v>
-      </c>
-      <c r="I23" s="163" t="s">
-        <v>34</v>
-      </c>
-      <c r="J23" s="163"/>
-      <c r="K23" s="163"/>
-      <c r="L23" s="163"/>
-      <c r="M23" s="162"/>
-      <c r="N23" s="164"/>
-      <c r="O23" s="165" t="s">
-        <v>34</v>
-      </c>
-      <c r="P23" s="166"/>
-      <c r="Q23" s="167"/>
-    </row>
-    <row r="24" spans="1:17" s="104" customFormat="1" ht="13.8" thickBot="1">
-      <c r="A24" s="168" t="s">
+      <c r="F23" s="158"/>
+      <c r="G23" s="159" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" s="160" t="s">
+        <v>34</v>
+      </c>
+      <c r="I23" s="161" t="s">
+        <v>34</v>
+      </c>
+      <c r="J23" s="161"/>
+      <c r="K23" s="161"/>
+      <c r="L23" s="161"/>
+      <c r="M23" s="160"/>
+      <c r="N23" s="162"/>
+      <c r="O23" s="163" t="s">
+        <v>34</v>
+      </c>
+      <c r="P23" s="164"/>
+      <c r="Q23" s="165"/>
+    </row>
+    <row r="24" spans="1:17" s="104" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A24" s="166" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="131" t="s">
@@ -2345,50 +2399,50 @@
       <c r="P24" s="138"/>
       <c r="Q24" s="139"/>
     </row>
-    <row r="25" spans="1:17" s="104" customFormat="1" ht="13.8" thickBot="1">
-      <c r="A25" s="169" t="s">
+    <row r="25" spans="1:17" s="104" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A25" s="167" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="170" t="s">
+      <c r="B25" s="168" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="170" t="s">
+      <c r="C25" s="168" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="170" t="s">
+      <c r="D25" s="168" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="171" t="s">
+      <c r="E25" s="169" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="172"/>
-      <c r="G25" s="173"/>
-      <c r="H25" s="174"/>
-      <c r="I25" s="174"/>
-      <c r="J25" s="174"/>
-      <c r="K25" s="174"/>
-      <c r="L25" s="174"/>
-      <c r="M25" s="174" t="s">
-        <v>34</v>
-      </c>
-      <c r="N25" s="175"/>
-      <c r="O25" s="176" t="s">
-        <v>34</v>
-      </c>
-      <c r="P25" s="177" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q25" s="178" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="13.8" thickTop="1"/>
-    <row r="28" spans="1:17" ht="16.2" thickBot="1">
+      <c r="F25" s="170"/>
+      <c r="G25" s="171"/>
+      <c r="H25" s="172"/>
+      <c r="I25" s="172"/>
+      <c r="J25" s="172"/>
+      <c r="K25" s="172"/>
+      <c r="L25" s="172"/>
+      <c r="M25" s="172" t="s">
+        <v>34</v>
+      </c>
+      <c r="N25" s="173"/>
+      <c r="O25" s="174" t="s">
+        <v>34</v>
+      </c>
+      <c r="P25" s="175" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q25" s="176" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="13.5" thickTop="1"/>
+    <row r="28" spans="1:17" ht="16.5" thickBot="1">
       <c r="A28" s="30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="16.8" thickTop="1" thickBot="1">
+    <row r="29" spans="1:17" ht="17.25" thickTop="1" thickBot="1">
       <c r="A29" s="16" t="s">
         <v>15</v>
       </c>
@@ -2439,7 +2493,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="14.4" thickTop="1" thickBot="1">
+    <row r="30" spans="1:17" ht="14.25" thickTop="1" thickBot="1">
       <c r="A30" s="44" t="s">
         <v>46</v>
       </c>
@@ -2476,7 +2530,7 @@
       <c r="P30" s="36"/>
       <c r="Q30" s="37"/>
     </row>
-    <row r="31" spans="1:17" ht="13.8" thickBot="1">
+    <row r="31" spans="1:17" ht="13.5" thickBot="1">
       <c r="A31" s="45" t="s">
         <v>50</v>
       </c>
@@ -2509,7 +2563,7 @@
       <c r="P31" s="24"/>
       <c r="Q31" s="25"/>
     </row>
-    <row r="32" spans="1:17" ht="13.8" thickBot="1">
+    <row r="32" spans="1:17" ht="13.5" thickBot="1">
       <c r="A32" s="43" t="s">
         <v>47</v>
       </c>
@@ -2544,18 +2598,18 @@
       </c>
       <c r="Q32" s="33"/>
     </row>
-    <row r="33" spans="1:17" ht="13.8" thickTop="1"/>
+    <row r="33" spans="1:17" ht="13.5" thickTop="1"/>
     <row r="34" spans="1:17">
       <c r="A34" s="46" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="104" customFormat="1" ht="16.2" thickBot="1">
+    <row r="37" spans="1:17" s="104" customFormat="1" ht="16.5" thickBot="1">
       <c r="A37" s="103" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="108" customFormat="1" ht="16.8" thickTop="1" thickBot="1">
+    <row r="38" spans="1:17" s="108" customFormat="1" ht="17.25" thickTop="1" thickBot="1">
       <c r="A38" s="105" t="s">
         <v>15</v>
       </c>
@@ -2606,7 +2660,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="104" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="39" spans="1:17" s="104" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A39" s="109" t="s">
         <v>63</v>
       </c>
@@ -2635,7 +2689,7 @@
       <c r="P39" s="117"/>
       <c r="Q39" s="118"/>
     </row>
-    <row r="40" spans="1:17" s="104" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="40" spans="1:17" s="104" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A40" s="109" t="s">
         <v>62</v>
       </c>
@@ -2666,7 +2720,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="104" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="41" spans="1:17" s="104" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A41" s="109" t="s">
         <v>61</v>
       </c>
@@ -2695,7 +2749,7 @@
       <c r="P41" s="126"/>
       <c r="Q41" s="127"/>
     </row>
-    <row r="42" spans="1:17" s="104" customFormat="1" ht="14.4" thickTop="1" thickBot="1">
+    <row r="42" spans="1:17" s="104" customFormat="1" ht="14.25" thickTop="1" thickBot="1">
       <c r="A42" s="128" t="s">
         <v>64</v>
       </c>
@@ -2724,7 +2778,7 @@
       <c r="P42" s="138"/>
       <c r="Q42" s="139"/>
     </row>
-    <row r="43" spans="1:17" s="104" customFormat="1" ht="14.4" thickTop="1" thickBot="1">
+    <row r="43" spans="1:17" s="104" customFormat="1" ht="14.25" thickTop="1" thickBot="1">
       <c r="A43" s="128" t="s">
         <v>65</v>
       </c>
@@ -2757,7 +2811,7 @@
       <c r="P43" s="138"/>
       <c r="Q43" s="139"/>
     </row>
-    <row r="44" spans="1:17" s="104" customFormat="1" ht="14.4" thickTop="1" thickBot="1">
+    <row r="44" spans="1:17" s="104" customFormat="1" ht="14.25" thickTop="1" thickBot="1">
       <c r="A44" s="128" t="s">
         <v>66</v>
       </c>
@@ -2790,7 +2844,7 @@
       <c r="P44" s="138"/>
       <c r="Q44" s="139"/>
     </row>
-    <row r="45" spans="1:17" s="104" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="45" spans="1:17" s="104" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A45" s="109" t="s">
         <v>67</v>
       </c>
@@ -2819,7 +2873,7 @@
       <c r="P45" s="126"/>
       <c r="Q45" s="127"/>
     </row>
-    <row r="46" spans="1:17" s="104" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="46" spans="1:17" s="104" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A46" s="109" t="s">
         <v>68</v>
       </c>
@@ -2850,7 +2904,7 @@
       </c>
       <c r="Q46" s="127"/>
     </row>
-    <row r="47" spans="1:17" s="104" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="47" spans="1:17" s="104" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A47" s="109" t="s">
         <v>69</v>
       </c>
@@ -2883,96 +2937,96 @@
       <c r="P47" s="126"/>
       <c r="Q47" s="127"/>
     </row>
-    <row r="48" spans="1:17" s="104" customFormat="1" ht="14.4" thickTop="1" thickBot="1">
-      <c r="A48" s="128" t="s">
+    <row r="48" spans="1:17" s="104" customFormat="1" ht="14.25" thickTop="1" thickBot="1">
+      <c r="A48" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="B48" s="129" t="s">
+      <c r="B48" s="179" t="s">
         <v>76</v>
       </c>
-      <c r="C48" s="130" t="s">
+      <c r="C48" s="69" t="s">
         <v>79</v>
       </c>
-      <c r="D48" s="131" t="s">
+      <c r="D48" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="E48" s="141" t="s">
+      <c r="E48" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="F48" s="142"/>
-      <c r="G48" s="134"/>
-      <c r="H48" s="135"/>
-      <c r="I48" s="135"/>
-      <c r="J48" s="135"/>
-      <c r="K48" s="135"/>
-      <c r="L48" s="135"/>
-      <c r="M48" s="135"/>
-      <c r="N48" s="143" t="s">
+      <c r="F48" s="180"/>
+      <c r="G48" s="181"/>
+      <c r="H48" s="77"/>
+      <c r="I48" s="77"/>
+      <c r="J48" s="77"/>
+      <c r="K48" s="77"/>
+      <c r="L48" s="77"/>
+      <c r="M48" s="77"/>
+      <c r="N48" s="79" t="s">
         <v>83</v>
       </c>
-      <c r="O48" s="137"/>
-      <c r="P48" s="138"/>
-      <c r="Q48" s="139"/>
-    </row>
-    <row r="49" spans="1:19" s="104" customFormat="1" ht="14.4" thickTop="1" thickBot="1">
-      <c r="A49" s="128" t="s">
+      <c r="O48" s="182"/>
+      <c r="P48" s="81"/>
+      <c r="Q48" s="80"/>
+    </row>
+    <row r="49" spans="1:19" s="104" customFormat="1" ht="14.25" thickTop="1" thickBot="1">
+      <c r="A49" s="178" t="s">
         <v>71</v>
       </c>
-      <c r="B49" s="129" t="s">
+      <c r="B49" s="183" t="s">
         <v>77</v>
       </c>
-      <c r="C49" s="130" t="s">
+      <c r="C49" s="69" t="s">
         <v>79</v>
       </c>
-      <c r="D49" s="131" t="s">
+      <c r="D49" s="184" t="s">
         <v>31</v>
       </c>
-      <c r="E49" s="141" t="s">
+      <c r="E49" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="F49" s="142"/>
-      <c r="G49" s="134"/>
-      <c r="H49" s="135"/>
-      <c r="I49" s="135"/>
-      <c r="J49" s="135"/>
-      <c r="K49" s="135"/>
-      <c r="L49" s="135"/>
-      <c r="M49" s="135"/>
-      <c r="N49" s="136"/>
-      <c r="O49" s="137"/>
-      <c r="P49" s="138"/>
-      <c r="Q49" s="144"/>
-    </row>
-    <row r="50" spans="1:19" s="104" customFormat="1" ht="14.4" thickTop="1" thickBot="1">
-      <c r="A50" s="128" t="s">
+      <c r="F49" s="180"/>
+      <c r="G49" s="71"/>
+      <c r="H49" s="72"/>
+      <c r="I49" s="72"/>
+      <c r="J49" s="72"/>
+      <c r="K49" s="72"/>
+      <c r="L49" s="72"/>
+      <c r="M49" s="72"/>
+      <c r="N49" s="73"/>
+      <c r="O49" s="74"/>
+      <c r="P49" s="75"/>
+      <c r="Q49" s="80"/>
+    </row>
+    <row r="50" spans="1:19" s="104" customFormat="1" ht="14.25" thickTop="1" thickBot="1">
+      <c r="A50" s="178" t="s">
         <v>72</v>
       </c>
-      <c r="B50" s="129" t="s">
+      <c r="B50" s="183" t="s">
         <v>78</v>
       </c>
-      <c r="C50" s="130" t="s">
+      <c r="C50" s="69" t="s">
         <v>80</v>
       </c>
-      <c r="D50" s="131" t="s">
+      <c r="D50" s="184" t="s">
         <v>31</v>
       </c>
-      <c r="E50" s="141" t="s">
+      <c r="E50" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="F50" s="142"/>
-      <c r="G50" s="134"/>
-      <c r="H50" s="135"/>
-      <c r="I50" s="135"/>
-      <c r="J50" s="135"/>
-      <c r="K50" s="135"/>
-      <c r="L50" s="135"/>
-      <c r="M50" s="135"/>
-      <c r="N50" s="136"/>
-      <c r="O50" s="137"/>
-      <c r="P50" s="145"/>
-      <c r="Q50" s="139"/>
-    </row>
-    <row r="51" spans="1:19" s="104" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="F50" s="180"/>
+      <c r="G50" s="71"/>
+      <c r="H50" s="72"/>
+      <c r="I50" s="72"/>
+      <c r="J50" s="72"/>
+      <c r="K50" s="72"/>
+      <c r="L50" s="72"/>
+      <c r="M50" s="72"/>
+      <c r="N50" s="73"/>
+      <c r="O50" s="74"/>
+      <c r="P50" s="81"/>
+      <c r="Q50" s="76"/>
+    </row>
+    <row r="51" spans="1:19" s="104" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A51" s="109" t="s">
         <v>73</v>
       </c>
@@ -3003,7 +3057,7 @@
       <c r="P51" s="126"/>
       <c r="Q51" s="127"/>
     </row>
-    <row r="52" spans="1:19" s="104" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="52" spans="1:19" s="104" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A52" s="109" t="s">
         <v>74</v>
       </c>
@@ -3032,36 +3086,36 @@
       <c r="P52" s="126"/>
       <c r="Q52" s="127"/>
     </row>
-    <row r="53" spans="1:19" s="104" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="53" spans="1:19" s="104" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A53" s="109" t="s">
         <v>75</v>
       </c>
       <c r="B53" s="110" t="s">
         <v>78</v>
       </c>
-      <c r="C53" s="146" t="s">
+      <c r="C53" s="144" t="s">
         <v>80</v>
       </c>
-      <c r="D53" s="146" t="s">
+      <c r="D53" s="144" t="s">
         <v>31</v>
       </c>
-      <c r="E53" s="147" t="s">
+      <c r="E53" s="145" t="s">
         <v>30</v>
       </c>
-      <c r="F53" s="148"/>
-      <c r="G53" s="149"/>
-      <c r="H53" s="150"/>
-      <c r="I53" s="150"/>
-      <c r="J53" s="150"/>
-      <c r="K53" s="150"/>
-      <c r="L53" s="150"/>
-      <c r="M53" s="150"/>
-      <c r="N53" s="151"/>
-      <c r="O53" s="152"/>
-      <c r="P53" s="153"/>
-      <c r="Q53" s="154"/>
-    </row>
-    <row r="54" spans="1:19" s="104" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="F53" s="146"/>
+      <c r="G53" s="147"/>
+      <c r="H53" s="148"/>
+      <c r="I53" s="148"/>
+      <c r="J53" s="148"/>
+      <c r="K53" s="148"/>
+      <c r="L53" s="148"/>
+      <c r="M53" s="148"/>
+      <c r="N53" s="149"/>
+      <c r="O53" s="150"/>
+      <c r="P53" s="151"/>
+      <c r="Q53" s="152"/>
+    </row>
+    <row r="54" spans="1:19" s="104" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A54" s="109" t="s">
         <v>84</v>
       </c>
@@ -3102,7 +3156,7 @@
       </c>
     </row>
     <row r="57" spans="1:19" s="104" customFormat="1">
-      <c r="A57" s="155" t="s">
+      <c r="A57" s="153" t="s">
         <v>85</v>
       </c>
       <c r="B57" s="104" t="s">
@@ -3111,15 +3165,15 @@
     </row>
     <row r="58" spans="1:19" s="104" customFormat="1">
       <c r="B58" s="104" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" s="54" customFormat="1" ht="16.2" thickBot="1">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" s="54" customFormat="1" ht="16.5" thickBot="1">
       <c r="A60" s="53" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="16.8" thickTop="1" thickBot="1">
+    <row r="61" spans="1:19" ht="17.25" thickTop="1" thickBot="1">
       <c r="A61" s="16" t="s">
         <v>15</v>
       </c>
@@ -3169,7 +3223,7 @@
         <v>38</v>
       </c>
       <c r="Q61" s="38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="R61" s="38" t="s">
         <v>90</v>
@@ -3178,9 +3232,9 @@
         <v>93</v>
       </c>
     </row>
-    <row r="62" spans="1:19" s="52" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="62" spans="1:19" s="52" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A62" s="99" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B62" s="83" t="s">
         <v>88</v>
@@ -3189,13 +3243,13 @@
         <v>79</v>
       </c>
       <c r="D62" s="100" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E62" s="56" t="s">
         <v>30</v>
       </c>
       <c r="F62" s="100" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G62" s="57"/>
       <c r="H62" s="58"/>
@@ -3215,9 +3269,9 @@
       <c r="R62" s="61"/>
       <c r="S62" s="61"/>
     </row>
-    <row r="63" spans="1:19" s="52" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="63" spans="1:19" s="52" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A63" s="99" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B63" s="83" t="s">
         <v>88</v>
@@ -3226,7 +3280,7 @@
         <v>79</v>
       </c>
       <c r="D63" s="100" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E63" s="63" t="s">
         <v>30</v>
@@ -3252,7 +3306,7 @@
       <c r="R63" s="68"/>
       <c r="S63" s="68"/>
     </row>
-    <row r="64" spans="1:19" s="52" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="64" spans="1:19" s="52" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A64" s="82" t="s">
         <v>87</v>
       </c>
@@ -3263,13 +3317,13 @@
         <v>79</v>
       </c>
       <c r="D64" s="100" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E64" s="63" t="s">
         <v>30</v>
       </c>
       <c r="F64" s="89" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G64" s="64"/>
       <c r="H64" s="65"/>
@@ -3289,9 +3343,9 @@
       <c r="R64" s="68"/>
       <c r="S64" s="68"/>
     </row>
-    <row r="65" spans="1:19" s="52" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="65" spans="1:19" s="52" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A65" s="99" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B65" s="83" t="s">
         <v>88</v>
@@ -3300,13 +3354,13 @@
         <v>79</v>
       </c>
       <c r="D65" s="100" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E65" s="78" t="s">
         <v>30</v>
       </c>
       <c r="F65" s="89" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G65" s="71"/>
       <c r="H65" s="72"/>
@@ -3326,9 +3380,9 @@
       </c>
       <c r="S65" s="80"/>
     </row>
-    <row r="66" spans="1:19" s="52" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="66" spans="1:19" s="52" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A66" s="99" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B66" s="83" t="s">
         <v>77</v>
@@ -3337,13 +3391,13 @@
         <v>79</v>
       </c>
       <c r="D66" s="100" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E66" s="70" t="s">
         <v>30</v>
       </c>
       <c r="F66" s="89" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G66" s="71"/>
       <c r="H66" s="72"/>
@@ -3363,9 +3417,9 @@
       <c r="R66" s="76"/>
       <c r="S66" s="76"/>
     </row>
-    <row r="67" spans="1:19" s="52" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="67" spans="1:19" s="52" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A67" s="99" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B67" s="83" t="s">
         <v>88</v>
@@ -3374,13 +3428,13 @@
         <v>80</v>
       </c>
       <c r="D67" s="100" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E67" s="70" t="s">
         <v>30</v>
       </c>
       <c r="F67" s="89" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G67" s="71" t="s">
         <v>34</v>
@@ -3400,9 +3454,9 @@
       <c r="R67" s="76"/>
       <c r="S67" s="76"/>
     </row>
-    <row r="68" spans="1:19" s="52" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="68" spans="1:19" s="52" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A68" s="99" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B68" s="83" t="s">
         <v>88</v>
@@ -3411,13 +3465,13 @@
         <v>80</v>
       </c>
       <c r="D68" s="100" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E68" s="63" t="s">
         <v>30</v>
       </c>
       <c r="F68" s="89" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G68" s="64"/>
       <c r="H68" s="65"/>
@@ -3437,9 +3491,9 @@
       <c r="R68" s="68"/>
       <c r="S68" s="68"/>
     </row>
-    <row r="69" spans="1:19" s="52" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="69" spans="1:19" s="52" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A69" s="99" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B69" s="83" t="s">
         <v>77</v>
@@ -3448,13 +3502,13 @@
         <v>79</v>
       </c>
       <c r="D69" s="100" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E69" s="78" t="s">
         <v>30</v>
       </c>
       <c r="F69" s="89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G69" s="71"/>
       <c r="H69" s="72"/>
@@ -3474,9 +3528,9 @@
       <c r="R69" s="76"/>
       <c r="S69" s="76"/>
     </row>
-    <row r="70" spans="1:19" s="52" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="70" spans="1:19" s="52" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A70" s="101" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B70" s="83" t="s">
         <v>77</v>
@@ -3485,13 +3539,13 @@
         <v>79</v>
       </c>
       <c r="D70" s="100" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E70" s="63" t="s">
         <v>30</v>
       </c>
       <c r="F70" s="89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G70" s="64"/>
       <c r="H70" s="65"/>
@@ -3511,9 +3565,9 @@
       <c r="R70" s="68"/>
       <c r="S70" s="68"/>
     </row>
-    <row r="71" spans="1:19" s="52" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="71" spans="1:19" s="52" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A71" s="99" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B71" s="83" t="s">
         <v>88</v>
@@ -3522,13 +3576,13 @@
         <v>80</v>
       </c>
       <c r="D71" s="100" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E71" s="78" t="s">
         <v>30</v>
       </c>
       <c r="F71" s="89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G71" s="71"/>
       <c r="H71" s="77" t="s">
@@ -3548,9 +3602,9 @@
       <c r="R71" s="76"/>
       <c r="S71" s="76"/>
     </row>
-    <row r="72" spans="1:19" s="52" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="72" spans="1:19" s="52" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A72" s="99" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B72" s="83" t="s">
         <v>88</v>
@@ -3559,13 +3613,13 @@
         <v>80</v>
       </c>
       <c r="D72" s="100" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E72" s="63" t="s">
         <v>30</v>
       </c>
       <c r="F72" s="89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G72" s="64"/>
       <c r="H72" s="65"/>
@@ -3585,24 +3639,24 @@
       <c r="R72" s="68"/>
       <c r="S72" s="68"/>
     </row>
-    <row r="73" spans="1:19" s="52" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="73" spans="1:19" s="52" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A73" s="99" t="s">
-        <v>119</v>
-      </c>
-      <c r="B73" s="179" t="s">
-        <v>123</v>
+        <v>118</v>
+      </c>
+      <c r="B73" s="177" t="s">
+        <v>122</v>
       </c>
       <c r="C73" s="69" t="s">
         <v>79</v>
       </c>
       <c r="D73" s="100" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E73" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="F73" s="89" t="s">
-        <v>95</v>
+      <c r="F73" s="185" t="s">
+        <v>124</v>
       </c>
       <c r="G73" s="71"/>
       <c r="H73" s="72"/>
@@ -3620,21 +3674,27 @@
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="13.8" thickBot="1"/>
-    <row r="76" spans="1:19" s="94" customFormat="1" ht="14.4" thickTop="1" thickBot="1">
+    <row r="74" spans="1:19" ht="15">
+      <c r="A74" s="186" t="s">
+        <v>123</v>
+      </c>
+      <c r="B74" s="187"/>
+    </row>
+    <row r="75" spans="1:19" ht="13.5" thickBot="1"/>
+    <row r="76" spans="1:19" s="94" customFormat="1" ht="14.25" thickTop="1" thickBot="1">
       <c r="A76" s="97" t="s">
         <v>89</v>
       </c>
       <c r="B76" s="98" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="77" spans="1:19" ht="15" thickTop="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" ht="15.75" thickTop="1">
       <c r="A77" s="95">
         <v>1</v>
       </c>
       <c r="B77" s="96" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="78" spans="1:19">
@@ -3642,7 +3702,7 @@
         <v>2</v>
       </c>
       <c r="B78" s="51" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="79" spans="1:19">
@@ -3650,30 +3710,33 @@
         <v>3</v>
       </c>
       <c r="B79" s="51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="80" spans="1:19">
       <c r="A80" s="51" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B80" s="51" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B81" s="51" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A62:S73">
     <sortCondition ref="F62:F73"/>
   </sortState>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <mergeCells count="1">
+    <mergeCell ref="A74:B74"/>
+  </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="41" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -3688,20 +3751,20 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
-    <col min="4" max="4" width="54.33203125" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="54.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.2" thickBot="1">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1">
       <c r="A1" s="30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" thickTop="1" thickBot="1">
+    <row r="2" spans="1:4" ht="17.25" thickTop="1" thickBot="1">
       <c r="A2" s="16" t="s">
         <v>15</v>
       </c>
@@ -3715,7 +3778,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.4" thickTop="1" thickBot="1">
+    <row r="3" spans="1:4" ht="14.25" thickTop="1" thickBot="1">
       <c r="A3" s="44" t="s">
         <v>51</v>
       </c>
@@ -3730,7 +3793,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated to reflect portal installation on trainingvm07.bmi.ohio-state.edu
</commit_message>
<xml_diff>
--- a/Documentation/management/osu/deployed_services.xlsx
+++ b/Documentation/management/osu/deployed_services.xlsx
@@ -386,20 +386,27 @@
     <t>portal</t>
   </si>
   <si>
-    <t>portal.training.cagrid.org now points to http://cagrid-portal.semanticbits.com/</t>
-  </si>
-  <si>
-    <t>none</t>
+    <t>trainingvm07.bmi.ohio-state.edu</t>
+  </si>
+  <si>
+    <t>portal.training.cagrid.org now points to http://trainingvm07.bmi.ohio-state.edu/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1033,12 +1040,12 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1071,12 +1078,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1096,15 +1103,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1113,66 +1120,66 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="29" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="26" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="27" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="28" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="14" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="23" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="24" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="26" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="27" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="28" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="20" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="23" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1188,112 +1195,112 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="30" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="26" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="27" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="27" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="28" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="20" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="23" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="23" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="24" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="30" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="13" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="26" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="27" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="27" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="28" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="20" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="23" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="23" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="24" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1311,34 +1318,34 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="31" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="17" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="21" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="25" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="25" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="22" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="31" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="21" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="25" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="25" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="22" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1350,7 +1357,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1379,30 +1386,30 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1707,7 +1714,7 @@
   <dimension ref="A2:S81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74:B74"/>
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3655,8 +3662,8 @@
       <c r="E73" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="F73" s="185" t="s">
-        <v>124</v>
+      <c r="F73" s="186" t="s">
+        <v>123</v>
       </c>
       <c r="G73" s="71"/>
       <c r="H73" s="72"/>
@@ -3675,10 +3682,10 @@
       </c>
     </row>
     <row r="74" spans="1:19" ht="15">
-      <c r="A74" s="186" t="s">
-        <v>123</v>
-      </c>
-      <c r="B74" s="187"/>
+      <c r="A74" s="187" t="s">
+        <v>124</v>
+      </c>
+      <c r="B74" s="185"/>
     </row>
     <row r="75" spans="1:19" ht="13.5" thickBot="1"/>
     <row r="76" spans="1:19" s="94" customFormat="1" ht="14.25" thickTop="1" thickBot="1">
@@ -3736,7 +3743,7 @@
   <mergeCells count="1">
     <mergeCell ref="A74:B74"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="41" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -3793,7 +3800,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>